<commit_message>
Data Provider code updated
</commit_message>
<xml_diff>
--- a/Data/DataSheet.xlsx
+++ b/Data/DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Reg ID" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>Test0001</t>
   </si>
@@ -54,10 +54,55 @@
     <t>JD000018</t>
   </si>
   <si>
-    <t>Web00420180000001930</t>
-  </si>
-  <si>
-    <t>Web00420180000001959</t>
+    <t>Web00420180000001938</t>
+  </si>
+  <si>
+    <t>UserID</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>AppID</t>
+  </si>
+  <si>
+    <t>Fname</t>
+  </si>
+  <si>
+    <t>Mname</t>
+  </si>
+  <si>
+    <t>Lname</t>
+  </si>
+  <si>
+    <t>Add</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Cpass</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Web00420180000001940</t>
+  </si>
+  <si>
+    <t>Web00420180000001941</t>
+  </si>
+  <si>
+    <t>Web00420180000001942</t>
   </si>
 </sst>
 </file>
@@ -65,7 +110,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,6 +124,14 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -105,10 +158,12 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -404,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -418,19 +473,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
-        <v>13</v>
+      <c r="C2" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
@@ -439,53 +505,86 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.140625" collapsed="true"/>
     <col min="9" max="9" customWidth="true" style="1" width="14.28515625" collapsed="true"/>
     <col min="10" max="10" bestFit="true" customWidth="true" width="21.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H2" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J2" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F1" r:id="rId1"/>
+    <hyperlink ref="F2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>

</xml_diff>